<commit_message>
updated COMPAS pidis deuteron data
</commit_message>
<xml_diff>
--- a/pidis/expdata/10001.xlsx
+++ b/pidis/expdata/10001.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jethier/Documents/fitpack/database/pdis/expdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fafd12/GIT/fitpack2/database/pidis/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA01D60-1A69-7C46-B044-B9E4A61F5B55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31380" windowHeight="17440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31380" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
   <si>
     <t>Elab</t>
   </si>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -133,6 +134,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -400,11 +404,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -458,10 +462,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="3">
-        <v>3.3E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="D2" s="3">
-        <v>0.78</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
@@ -470,21 +474,21 @@
         <v>12</v>
       </c>
       <c r="G2" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>-5.4000000000000003E-3</v>
       </c>
       <c r="H2" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>7.4000000000000003E-3</v>
       </c>
       <c r="I2" s="3">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="J2" s="3">
-        <f t="shared" ref="J2:J18" si="0">G2/10</f>
-        <v>3.0000000000000003E-4</v>
+        <f>G2/10</f>
+        <v>-5.4000000000000001E-4</v>
       </c>
       <c r="K2" s="1">
-        <f t="shared" ref="K2:K18" si="1">MAX(I2^2-J2^2,0)^0.5</f>
-        <v>3.9887341350358261E-3</v>
+        <f>MAX(I2^2-J2^2,0)^0.5</f>
+        <v>4.7695282785617278E-3</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -498,10 +502,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="3">
-        <v>3.8E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="D3" s="3">
-        <v>0.83</v>
+        <v>1.22</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
@@ -510,21 +514,21 @@
         <v>12</v>
       </c>
       <c r="G3" s="3">
-        <v>-4.0000000000000001E-3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="H3" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="I3" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" si="0"/>
-        <v>-4.0000000000000002E-4</v>
+        <f t="shared" ref="J3:J16" si="0">G3/10</f>
+        <v>2.9999999999999997E-5</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" si="1"/>
-        <v>2.9732137494637013E-3</v>
+        <f t="shared" ref="K2:K16" si="1">MAX(I3^2-J3^2,0)^0.5</f>
+        <v>4.2998953475637059E-3</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>10</v>
@@ -538,10 +542,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>4.5999999999999999E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D4" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.39</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
@@ -550,21 +554,21 @@
         <v>12</v>
       </c>
       <c r="G4" s="3">
-        <v>4.0000000000000001E-3</v>
+        <v>-1.1000000000000001E-3</v>
       </c>
       <c r="H4" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="I4" s="3">
-        <v>4.0000000000000001E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" si="0"/>
-        <v>4.0000000000000002E-4</v>
+        <v>-1.1E-4</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="1"/>
-        <v>3.9799497484264796E-3</v>
+        <v>2.297368059323538E-3</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>10</v>
@@ -578,10 +582,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>5.4999999999999997E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D5" s="3">
-        <v>1.22</v>
+        <v>1.62</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
@@ -590,21 +594,21 @@
         <v>12</v>
       </c>
       <c r="G5" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>-8.6999999999999994E-3</v>
       </c>
       <c r="H5" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="I5" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="0"/>
-        <v>3.0000000000000003E-4</v>
+        <v>-8.699999999999999E-4</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="1"/>
-        <v>2.9849623113198599E-3</v>
+        <v>2.9754159373102779E-3</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>10</v>
@@ -618,10 +622,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>1.41E-2</v>
       </c>
       <c r="D6" s="3">
-        <v>1.39</v>
+        <v>2.19</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
@@ -630,21 +634,21 @@
         <v>12</v>
       </c>
       <c r="G6" s="3">
-        <v>-2E-3</v>
+        <v>-1.1000000000000001E-3</v>
       </c>
       <c r="H6" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="I6" s="3">
-        <v>2E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>-2.0000000000000001E-4</v>
+        <v>-1.1E-4</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="1"/>
-        <v>1.9899748742132398E-3</v>
+        <v>2.3974778413991646E-3</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>10</v>
@@ -658,10 +662,10 @@
         <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>2.4400000000000002E-2</v>
       </c>
       <c r="D7" s="3">
-        <v>1.61</v>
+        <v>3.29</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
@@ -670,21 +674,21 @@
         <v>12</v>
       </c>
       <c r="G7" s="3">
-        <v>-0.01</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="H7" s="3">
-        <v>6.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="I7" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>-1E-3</v>
+        <v>7.5000000000000002E-4</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="1"/>
-        <v>2.8284271247461901E-3</v>
+        <v>3.3162478797580859E-3</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>10</v>
@@ -698,10 +702,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="3">
-        <v>1.41E-2</v>
+        <v>3.4599999999999999E-2</v>
       </c>
       <c r="D8" s="3">
-        <v>2.15</v>
+        <v>4.43</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
@@ -710,21 +714,21 @@
         <v>12</v>
       </c>
       <c r="G8" s="3">
-        <v>2E-3</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="H8" s="3">
-        <v>4.0000000000000001E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="I8" s="3">
-        <v>2E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>2.0000000000000001E-4</v>
+        <v>9.5E-4</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="1"/>
-        <v>1.9899748742132398E-3</v>
+        <v>4.0911489828653266E-3</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>10</v>
@@ -738,10 +742,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="3">
-        <v>2.4400000000000002E-2</v>
+        <v>4.87E-2</v>
       </c>
       <c r="D9" s="3">
-        <v>3.18</v>
+        <v>6.06</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>11</v>
@@ -750,21 +754,21 @@
         <v>12</v>
       </c>
       <c r="G9" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="H9" s="3">
-        <v>6.0000000000000001E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="I9" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>3.0000000000000003E-4</v>
+        <v>1.5900000000000001E-3</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="1"/>
-        <v>2.9849623113198599E-3</v>
+        <v>4.1026698624188618E-3</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>10</v>
@@ -778,10 +782,10 @@
         <v>10</v>
       </c>
       <c r="C10" s="3">
-        <v>3.4599999999999999E-2</v>
+        <v>7.6600000000000001E-2</v>
       </c>
       <c r="D10" s="3">
-        <v>4.26</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
@@ -790,21 +794,21 @@
         <v>12</v>
       </c>
       <c r="G10" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>5.2699999999999997E-2</v>
       </c>
       <c r="H10" s="3">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="I10" s="3">
-        <v>4.0000000000000001E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>8.9999999999999998E-4</v>
+        <v>5.2699999999999995E-3</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="1"/>
-        <v>3.8974350539810153E-3</v>
+        <v>4.9058230705968193E-3</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>10</v>
@@ -818,10 +822,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="3">
-        <v>4.87E-2</v>
+        <v>0.121</v>
       </c>
       <c r="D11" s="3">
-        <v>5.8</v>
+        <v>13.5</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>11</v>
@@ -830,21 +834,21 @@
         <v>12</v>
       </c>
       <c r="G11" s="3">
-        <v>1.7000000000000001E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="H11" s="3">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="I11" s="3">
-        <v>4.0000000000000001E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="0"/>
-        <v>1.7000000000000001E-3</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="1"/>
-        <v>3.620773398046334E-3</v>
+        <v>5.545268253204708E-3</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>10</v>
@@ -858,10 +862,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="3">
-        <v>7.6499999999999999E-2</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="D12" s="3">
-        <v>8.5299999999999994</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>11</v>
@@ -870,21 +874,21 @@
         <v>12</v>
       </c>
       <c r="G12" s="3">
-        <v>5.8000000000000003E-2</v>
+        <v>0.121</v>
       </c>
       <c r="H12" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I12" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="0"/>
-        <v>5.8000000000000005E-3</v>
+        <v>1.21E-2</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="1"/>
-        <v>3.9191835884530854E-3</v>
+        <v>1.0468524251297314E-2</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>10</v>
@@ -898,10 +902,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="3">
-        <v>0.121</v>
+        <v>0.222</v>
       </c>
       <c r="D13" s="3">
-        <v>12.6</v>
+        <v>23.8</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>11</v>
@@ -910,21 +914,21 @@
         <v>12</v>
       </c>
       <c r="G13" s="3">
-        <v>9.5000000000000001E-2</v>
+        <v>0.16</v>
       </c>
       <c r="H13" s="3">
-        <v>1.2999999999999999E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I13" s="3">
-        <v>1.0999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="0"/>
-        <v>9.4999999999999998E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="K13" s="1">
         <f t="shared" si="1"/>
-        <v>5.545268253204708E-3</v>
+        <v>1.2000000000000002E-2</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>10</v>
@@ -938,10 +942,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="3">
-        <v>0.17100000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D14" s="3">
-        <v>17.2</v>
+        <v>31.1</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>11</v>
@@ -950,21 +954,21 @@
         <v>12</v>
       </c>
       <c r="G14" s="3">
-        <v>0.123</v>
+        <v>0.19</v>
       </c>
       <c r="H14" s="3">
-        <v>0.02</v>
+        <v>2.3E-2</v>
       </c>
       <c r="I14" s="3">
-        <v>1.4E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="0"/>
-        <v>1.23E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="1"/>
-        <v>6.6865536713616551E-3</v>
+        <v>1.1090536506409416E-2</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>10</v>
@@ -978,10 +982,10 @@
         <v>10</v>
       </c>
       <c r="C15" s="3">
-        <v>0.222</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="D15" s="3">
-        <v>21.8</v>
+        <v>43.9</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>11</v>
@@ -990,21 +994,21 @@
         <v>12</v>
       </c>
       <c r="G15" s="3">
-        <v>0.183</v>
+        <v>0.317</v>
       </c>
       <c r="H15" s="3">
-        <v>2.8000000000000001E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="I15" s="3">
-        <v>2.1000000000000001E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="0"/>
-        <v>1.83E-2</v>
+        <v>3.1699999999999999E-2</v>
       </c>
       <c r="K15" s="1">
         <f t="shared" si="1"/>
-        <v>1.0300970828033638E-2</v>
+        <v>1.7061945961700846E-2</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>10</v>
@@ -1018,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="D16" s="3">
-        <v>28.3</v>
+        <v>60.8</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>11</v>
@@ -1030,103 +1034,23 @@
         <v>12</v>
       </c>
       <c r="G16" s="3">
-        <v>0.216</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="H16" s="3">
-        <v>0.03</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="I16" s="3">
-        <v>2.4E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="0"/>
-        <v>2.1600000000000001E-2</v>
+        <v>4.9399999999999999E-2</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" si="1"/>
-        <v>1.0461357464497615E-2</v>
+        <v>6.7938501602552298E-2</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="3">
-        <v>160</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="D17" s="3">
-        <v>39.700000000000003</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="H17" s="3">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="I17" s="3">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" si="0"/>
-        <v>3.4300000000000004E-2</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6355732939859334E-2</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="3">
-        <v>160</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D18" s="3">
-        <v>55.3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.626</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0.112</v>
-      </c>
-      <c r="I18" s="3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="0"/>
-        <v>6.2600000000000003E-2</v>
-      </c>
-      <c r="K18" s="1">
-        <f t="shared" si="1"/>
-        <v>4.1306658058961866E-2</v>
-      </c>
-      <c r="L18" s="4" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>